<commit_message>
Escribir Excel con datos del formulario
</commit_message>
<xml_diff>
--- a/PDF-Filler/OutputExcelFiles/imm5713e.xlsx
+++ b/PDF-Filler/OutputExcelFiles/imm5713e.xlsx
@@ -12,87 +12,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>familyName</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>givenName</t>
+  </si>
+  <si>
+    <t>theDate</t>
+  </si>
+  <si>
+    <t>1/1/0001 00:00:00</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>TextField1</t>
+  </si>
+  <si>
+    <t>DateTimeField1</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
   <si>
     <t>{</t>
   </si>
   <si>
-    <t>"</t>
+    <t>v</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
   <si>
     <t>f</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>c</t>
@@ -147,7 +174,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A250"/>
+  <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -157,1250 +184,1286 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>